<commit_message>
Update help hours in schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
   <si>
     <t>Time</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Help Hours</t>
+  </si>
+  <si>
+    <t>Help Hours*</t>
   </si>
 </sst>
 </file>
@@ -453,7 +456,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +580,7 @@
         <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>29</v>
@@ -591,7 +594,7 @@
         <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Update pages for S25
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="11475" windowHeight="7755"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="11475" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="My Schedule" sheetId="1" r:id="rId1"/>
+    <sheet name="STT 1810" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="42">
   <si>
     <t>Time</t>
   </si>
@@ -102,16 +102,46 @@
     <t>07:30-08:00</t>
   </si>
   <si>
-    <t>STT 4811</t>
-  </si>
-  <si>
     <t>STT 1810</t>
   </si>
   <si>
     <t>Help Hours</t>
   </si>
   <si>
-    <t>Help Hours*</t>
+    <t>STT 4812</t>
+  </si>
+  <si>
+    <t>09:00-09:30</t>
+  </si>
+  <si>
+    <t>09:30-10:00</t>
+  </si>
+  <si>
+    <t>XXXXX</t>
+  </si>
+  <si>
+    <t>Dept Meetings</t>
+  </si>
+  <si>
+    <t>Jill =</t>
+  </si>
+  <si>
+    <t>Molly =</t>
+  </si>
+  <si>
+    <t>Lisa =</t>
+  </si>
+  <si>
+    <t>T/R at 11:00 am to 1:45 pm, 3:30 pm to 4:45 pm</t>
+  </si>
+  <si>
+    <t>M/W/F at 10:00 am to 10:50 am, 12:00 pm to 12:50 pm</t>
+  </si>
+  <si>
+    <t>W at 9:00 to 9:50 am, 11:00 am to 11:50 am</t>
+  </si>
+  <si>
+    <t>T/R at 9:30 am to 10:45 am, 11:00 am to 12:15 pm, 2:00 pm to 3:15 pm</t>
   </si>
 </sst>
 </file>
@@ -147,10 +177,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -455,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,21 +524,33 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>17</v>
@@ -513,10 +561,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>17</v>
@@ -526,6 +574,12 @@
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F6" s="1" t="s">
         <v>17</v>
       </c>
@@ -535,10 +589,10 @@
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>17</v>
@@ -549,10 +603,10 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>17</v>
@@ -563,10 +617,10 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>17</v>
@@ -579,9 +633,6 @@
       <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E10" s="1" t="s">
         <v>29</v>
       </c>
@@ -593,9 +644,6 @@
       <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E11" s="1" t="s">
         <v>29</v>
       </c>
@@ -604,14 +652,8 @@
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="D12" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -619,13 +661,13 @@
         <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -633,13 +675,13 @@
         <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -647,24 +689,27 @@
         <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -675,7 +720,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -686,7 +731,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -697,7 +742,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -708,7 +753,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -726,12 +771,297 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="6" width="15.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add math ed meeting time
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoml\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DC82BF-4E62-40EA-8E2D-473FD3204FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="My Schedule" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
   <si>
     <t>Time</t>
   </si>
@@ -124,7 +118,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -177,9 +171,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -217,7 +211,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -289,7 +283,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -462,11 +456,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,6 +515,9 @@
       <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>28</v>
       </c>
@@ -534,6 +531,9 @@
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Update webpage for S26
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomleyje\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3720343D-CF76-453B-A258-7481CD1FE9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="My Schedule" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t>Time</t>
   </si>
@@ -100,25 +106,25 @@
     <t>07:30-08:00</t>
   </si>
   <si>
-    <t>STT 1810</t>
-  </si>
-  <si>
     <t>Help Hours</t>
   </si>
   <si>
-    <t>STT 4811</t>
-  </si>
-  <si>
     <t>9:00-9:30</t>
   </si>
   <si>
     <t>9:30-10:00</t>
+  </si>
+  <si>
+    <t>STT 4812</t>
+  </si>
+  <si>
+    <t>STT 5811</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -171,9 +177,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -211,7 +217,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -283,7 +289,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -456,11 +462,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,12 +496,12 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -512,15 +518,6 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F6" s="1" t="s">
         <v>17</v>
       </c>
@@ -529,15 +526,6 @@
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F7" s="1" t="s">
         <v>17</v>
       </c>
@@ -546,12 +534,6 @@
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" s="1" t="s">
         <v>17</v>
       </c>
@@ -561,10 +543,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>17</v>
@@ -575,10 +557,10 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>17</v>
@@ -589,10 +571,10 @@
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>17</v>
@@ -603,10 +585,10 @@
         <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -614,10 +596,10 @@
         <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -625,13 +607,13 @@
         <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -639,13 +621,13 @@
         <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -653,13 +635,13 @@
         <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -667,27 +649,21 @@
         <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -698,12 +674,9 @@
         <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D19"/>
-      <c r="E19" s="1" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -723,6 +696,9 @@
       <c r="B21" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
@@ -734,6 +710,9 @@
       <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C22" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22"/>
@@ -743,6 +722,9 @@
         <v>27</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D23"/>

</xml_diff>

<commit_message>
Add THU office hours
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomleyje\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3720343D-CF76-453B-A258-7481CD1FE9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="My Schedule" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
   <si>
     <t>Time</t>
   </si>
@@ -124,7 +118,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -177,9 +171,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -217,7 +211,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -289,7 +283,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -462,11 +456,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,6 +659,9 @@
       <c r="C18" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="E18" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -677,6 +674,9 @@
         <v>17</v>
       </c>
       <c r="D19"/>
+      <c r="E19" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">

</xml_diff>